<commit_message>
turning in what I have
</commit_message>
<xml_diff>
--- a/Prove-Assignments/Predictions Ponder-Prove-05.xlsx
+++ b/Prove-Assignments/Predictions Ponder-Prove-05.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/771c9d6cd312e0e1/BYUI/CS450 (Machine Learning)/machine-learning/Prove-Assignments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="8_{E05E2EFB-837D-4456-873A-F3F7CE9A75DC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{0BAE1401-33E4-4BBE-B0CF-624CAB758372}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="8_{E05E2EFB-837D-4456-873A-F3F7CE9A75DC}" xr6:coauthVersionLast="29" xr6:coauthVersionMax="29" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="23040" windowHeight="9036" xr2:uid="{75A53DAA-2034-40E0-927C-3F841B318330}"/>
+    <workbookView xWindow="0" yWindow="4200" windowWidth="23040" windowHeight="9036" xr2:uid="{75A53DAA-2034-40E0-927C-3F841B318330}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179016"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="61">
+  <si>
+    <t>CS 450 05-Prove</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>CreditScore:</t>
+  </si>
+  <si>
+    <t>Income:</t>
+  </si>
+  <si>
+    <t>Collateral:</t>
+  </si>
+  <si>
+    <t>Job History:</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Poor</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Data Table</t>
+  </si>
+  <si>
+    <t>Probabilities</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
   <si>
     <t>Credit Score</t>
   </si>
@@ -42,92 +90,134 @@
     <t>Job History</t>
   </si>
   <si>
-    <t>Good</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Short</t>
+    <t xml:space="preserve">Should Loan </t>
+  </si>
+  <si>
+    <t>Class Count:</t>
+  </si>
+  <si>
+    <t>Class Conditionals:</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>Long</t>
-  </si>
-  <si>
-    <t>Poor</t>
+    <t>Should Loan</t>
+  </si>
+  <si>
+    <t>Credit Score (Good)</t>
+  </si>
+  <si>
+    <t>Credit Score (Average)</t>
+  </si>
+  <si>
+    <t>Credit Score (Low)</t>
+  </si>
+  <si>
+    <t>Likelihood (Yes/No)</t>
+  </si>
+  <si>
+    <t>Credit Score (good)</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>CS 450 05-Prove</t>
-  </si>
-  <si>
-    <t>Row</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Should Loan </t>
-  </si>
-  <si>
-    <t>Probabilities</t>
-  </si>
-  <si>
-    <t>Legend</t>
-  </si>
-  <si>
-    <t>CreditScore:</t>
-  </si>
-  <si>
-    <t>Income:</t>
-  </si>
-  <si>
-    <t>Collateral:</t>
-  </si>
-  <si>
-    <t>Job History:</t>
-  </si>
-  <si>
-    <t>Credit Score (good)</t>
-  </si>
-  <si>
-    <t>Credit Score (Average)</t>
-  </si>
-  <si>
-    <t>Credit Score (Low)</t>
-  </si>
-  <si>
-    <t>P(</t>
-  </si>
-  <si>
-    <t>hi</t>
-  </si>
-  <si>
-    <t>coll</t>
-  </si>
-  <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>Should Loan</t>
-  </si>
-  <si>
-    <t>should loan = dependent</t>
+    <t>Income (High)</t>
+  </si>
+  <si>
+    <t>Income (Low)</t>
+  </si>
+  <si>
+    <t>Collateral (Good)</t>
+  </si>
+  <si>
+    <t>Collateral (Poor)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Job History (Long) </t>
+  </si>
+  <si>
+    <t>Job History (Short)</t>
+  </si>
+  <si>
+    <t>Instances:</t>
+  </si>
+  <si>
+    <t>P(yes| Credit Score) = 8</t>
+  </si>
+  <si>
+    <t>1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P(Yes) * P(Credit Score | Good) * P(Income | High) * P(Collateral | Good) * P(Job History | Long) </t>
+  </si>
+  <si>
+    <t>P(no| Credit Score) = 6</t>
+  </si>
+  <si>
+    <t>P(No) * P(Credit Score | Good) * P(Income | High) * P(Collateral | Good) * P(Job History | Long)</t>
+  </si>
+  <si>
+    <t>P(yes| Income) = 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P(Yes) </t>
+  </si>
+  <si>
+    <t>Answer: yes</t>
+  </si>
+  <si>
+    <t>P(no| Income) = 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P(No) </t>
+  </si>
+  <si>
+    <t>P(yes| Collateral) = 6</t>
+  </si>
+  <si>
+    <t>2)</t>
+  </si>
+  <si>
+    <t>P(Yes) * P(Credit Score | Average) * P(Income | Low) * P(Collateral | Good) * P(Job History | Short) </t>
+  </si>
+  <si>
+    <t>P(no| Collateral = 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P(No) * P(Credit Score | Average) * P(Income | Low) * P(Collateral | Good) * P(Job History | Short) </t>
+  </si>
+  <si>
+    <t>P(yes| Job History) = 6</t>
+  </si>
+  <si>
+    <t>Answer: No</t>
+  </si>
+  <si>
+    <t>P(no| Job History) = 8</t>
+  </si>
+  <si>
+    <t>P(yes) = 6</t>
+  </si>
+  <si>
+    <t>3)</t>
+  </si>
+  <si>
+    <t>P(Yes) * P(Credit Score | Low) * P(Income | High) * P(Collateral | Poor) * P(Job History | Short )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P(No) = 8 </t>
+  </si>
+  <si>
+    <t>P(No) * P(Credit Score | Low) * P(Income | High) * P(Collateral | Poor) * P(Job History | Short )</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="12">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,8 +305,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,8 +347,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -262,13 +384,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -277,11 +446,27 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="3"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="4"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -289,13 +474,31 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="4" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Calculation" xfId="3" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,591 +863,1127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55B4E4-6041-4A0E-8421-36179B47D012}">
-  <dimension ref="B6:BC33"/>
+  <dimension ref="B6:BD55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0" xr3:uid="{984E07D0-8CAE-5625-9A34-D8B9FA7103F7}">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
     <col min="8" max="8" width="6" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" customWidth="1"/>
-    <col min="10" max="10" width="18.77734375" customWidth="1"/>
-    <col min="11" max="11" width="24.21875" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" customWidth="1"/>
-    <col min="13" max="13" width="17.21875" customWidth="1"/>
-    <col min="14" max="14" width="21.109375" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="24.28515625" customWidth="1"/>
+    <col min="12" max="13" width="19.28515625" customWidth="1"/>
+    <col min="14" max="14" width="5.5703125" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" customWidth="1"/>
+    <col min="17" max="17" width="25.28515625" customWidth="1"/>
+    <col min="18" max="18" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:55" ht="15" thickBot="1">
-      <c r="B6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="2:55" ht="15.6" thickTop="1" thickBot="1">
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="2:55" ht="15.6" thickTop="1" thickBot="1">
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="2:55" ht="15" thickTop="1"/>
-    <row r="10" spans="2:55">
-      <c r="B10" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="2:55" ht="14.4" customHeight="1">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="2:55">
-      <c r="B12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>21</v>
+    <row r="6" spans="2:56" ht="15" thickBot="1">
+      <c r="B6" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+    </row>
+    <row r="7" spans="2:56" ht="15.6" thickTop="1" thickBot="1">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="2:56" ht="15.6" thickTop="1" thickBot="1">
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="2:56" ht="15" thickTop="1"/>
+    <row r="10" spans="2:56">
+      <c r="B10" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="2:56" ht="14.45" customHeight="1">
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+    </row>
+    <row r="12" spans="2:56">
+      <c r="B12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="2:55" ht="21" customHeight="1">
+    <row r="13" spans="2:56" ht="21" customHeight="1">
       <c r="B13" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
       </c>
-      <c r="J13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="2:55" ht="19.2" customHeight="1">
+    </row>
+    <row r="14" spans="2:56" ht="19.149999999999999" customHeight="1">
       <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="2:55" ht="17.399999999999999" customHeight="1">
+    </row>
+    <row r="15" spans="2:56" ht="17.45" customHeight="1">
       <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="AX15" s="1"/>
+        <v>10</v>
+      </c>
       <c r="AY15" s="1"/>
       <c r="AZ15" s="1"/>
       <c r="BA15" s="1"/>
       <c r="BB15" s="1"/>
       <c r="BC15" s="1"/>
-    </row>
-    <row r="16" spans="2:55" ht="18.600000000000001" customHeight="1">
-      <c r="AX16" s="2"/>
+      <c r="BD15" s="1"/>
+    </row>
+    <row r="16" spans="2:56" ht="18.600000000000001" customHeight="1">
       <c r="AY16" s="2"/>
       <c r="AZ16" s="2"/>
       <c r="BA16" s="2"/>
       <c r="BB16" s="2"/>
       <c r="BC16" s="2"/>
-    </row>
-    <row r="17" spans="2:55" ht="19.2" customHeight="1">
-      <c r="I17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="AX17" s="2"/>
+      <c r="BD16" s="2"/>
+    </row>
+    <row r="17" spans="2:56" ht="19.149999999999999" customHeight="1">
+      <c r="B17" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="I17" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
       <c r="AY17" s="2"/>
       <c r="AZ17" s="2"/>
       <c r="BA17" s="2"/>
       <c r="BB17" s="2"/>
       <c r="BC17" s="2"/>
-    </row>
-    <row r="18" spans="2:55" ht="15" customHeight="1">
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="AX18" s="2"/>
+      <c r="BD17" s="2"/>
+    </row>
+    <row r="18" spans="2:56" ht="15" customHeight="1" thickBot="1">
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
       <c r="AY18" s="2"/>
       <c r="AZ18" s="2"/>
       <c r="BA18" s="2"/>
       <c r="BB18" s="2"/>
       <c r="BC18" s="2"/>
-    </row>
-    <row r="19" spans="2:55" ht="16.8">
+      <c r="BD18" s="2"/>
+    </row>
+    <row r="19" spans="2:56" ht="18" thickTop="1" thickBot="1">
       <c r="B19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="F19" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" t="s">
-        <v>29</v>
-      </c>
-      <c r="J19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="O19" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="K19" t="s">
-        <v>23</v>
-      </c>
-      <c r="L19" t="s">
-        <v>24</v>
-      </c>
-      <c r="AX19" s="2"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="7"/>
       <c r="AY19" s="2"/>
       <c r="AZ19" s="2"/>
       <c r="BA19" s="2"/>
       <c r="BB19" s="2"/>
       <c r="BC19" s="2"/>
-    </row>
-    <row r="20" spans="2:55" ht="17.399999999999999" customHeight="1">
+      <c r="BD19" s="2"/>
+    </row>
+    <row r="20" spans="2:56" ht="17.45" customHeight="1" thickTop="1" thickBot="1">
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F20" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>7</v>
-      </c>
-      <c r="I20" t="s">
-        <v>5</v>
-      </c>
-      <c r="J20">
-        <v>3</v>
-      </c>
-      <c r="K20">
-        <v>2</v>
-      </c>
-      <c r="L20">
-        <v>3</v>
-      </c>
-      <c r="AX20" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P20" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R20" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="AY20" s="2"/>
       <c r="AZ20" s="2"/>
       <c r="BA20" s="2"/>
       <c r="BB20" s="2"/>
       <c r="BC20" s="2"/>
-    </row>
-    <row r="21" spans="2:55" ht="16.8" customHeight="1">
+      <c r="BD20" s="2"/>
+    </row>
+    <row r="21" spans="2:56" ht="16.899999999999999" customHeight="1" thickTop="1" thickBot="1">
       <c r="B21">
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F21" t="s">
         <v>8</v>
       </c>
       <c r="G21" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" t="s">
-        <v>11</v>
-      </c>
-      <c r="J21">
+        <v>23</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="9">
+        <v>3</v>
+      </c>
+      <c r="K21" s="9">
         <v>2</v>
       </c>
-      <c r="K21">
-        <v>3</v>
-      </c>
-      <c r="L21">
+      <c r="L21" s="9">
         <v>1</v>
       </c>
-      <c r="AX21" s="2"/>
+      <c r="M21" s="9">
+        <f>SUM(J21+K21+L21)</f>
+        <v>6</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="P21" s="7">
+        <f>3/5</f>
+        <v>0.6</v>
+      </c>
+      <c r="Q21" s="7">
+        <f>2/5</f>
+        <v>0.4</v>
+      </c>
+      <c r="R21" s="7">
+        <f>L21/4</f>
+        <v>0.25</v>
+      </c>
       <c r="AY21" s="2"/>
       <c r="AZ21" s="2"/>
       <c r="BA21" s="2"/>
       <c r="BB21" s="2"/>
       <c r="BC21" s="2"/>
-    </row>
-    <row r="22" spans="2:55" ht="18.600000000000001" customHeight="1">
+      <c r="BD21" s="2"/>
+    </row>
+    <row r="22" spans="2:56" ht="18.600000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="B22">
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="s">
+        <v>30</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J22" s="9">
+        <v>2</v>
+      </c>
+      <c r="K22" s="9">
+        <v>3</v>
+      </c>
+      <c r="L22" s="9">
+        <v>1</v>
+      </c>
+      <c r="M22" s="9">
+        <f>SUM(J22+K22+L22)</f>
         <v>6</v>
       </c>
-      <c r="G22" t="s">
-        <v>10</v>
-      </c>
-      <c r="AX22" s="2"/>
+      <c r="O22" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P22" s="7">
+        <f>2/6</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Q22" s="7">
+        <f>3/5</f>
+        <v>0.6</v>
+      </c>
+      <c r="R22" s="7">
+        <f>L22/4</f>
+        <v>0.25</v>
+      </c>
       <c r="AY22" s="2"/>
       <c r="AZ22" s="2"/>
       <c r="BA22" s="2"/>
       <c r="BB22" s="2"/>
       <c r="BC22" s="2"/>
-    </row>
-    <row r="23" spans="2:55" ht="18.600000000000001" customHeight="1">
+      <c r="BD22" s="2"/>
+    </row>
+    <row r="23" spans="2:56" ht="18.600000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="B23">
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F23" t="s">
         <v>8</v>
       </c>
       <c r="G23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I23" t="s">
-        <v>1</v>
-      </c>
-      <c r="J23" t="s">
-        <v>27</v>
-      </c>
-      <c r="AX23" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
       <c r="AY23" s="2"/>
       <c r="AZ23" s="2"/>
       <c r="BA23" s="2"/>
       <c r="BB23" s="2"/>
       <c r="BC23" s="2"/>
-    </row>
-    <row r="24" spans="2:55" ht="18.600000000000001" customHeight="1">
+      <c r="BD23" s="2"/>
+    </row>
+    <row r="24" spans="2:56" ht="18.600000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="B24">
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
         <v>11</v>
-      </c>
-      <c r="E24" t="s">
-        <v>9</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>
       </c>
       <c r="G24" t="s">
-        <v>10</v>
-      </c>
-      <c r="I24" t="s">
-        <v>26</v>
-      </c>
-      <c r="AX24" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="O24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P24" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q24" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="R24" s="7"/>
       <c r="AY24" s="2"/>
       <c r="AZ24" s="2"/>
       <c r="BA24" s="2"/>
       <c r="BB24" s="2"/>
       <c r="BC24" s="2"/>
-    </row>
-    <row r="25" spans="2:55" ht="16.8">
+      <c r="BD24" s="2"/>
+    </row>
+    <row r="25" spans="2:56" ht="18" thickTop="1" thickBot="1">
       <c r="B25">
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F25" t="s">
         <v>8</v>
       </c>
       <c r="G25" t="s">
-        <v>7</v>
-      </c>
-      <c r="I25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AX25" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" s="9">
+        <v>5</v>
+      </c>
+      <c r="K25" s="9">
+        <v>1</v>
+      </c>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9">
+        <f t="shared" ref="M25:M34" si="0">SUM(J25+K25+L25)</f>
+        <v>6</v>
+      </c>
+      <c r="O25" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="P25" s="7">
+        <f>J25/8</f>
+        <v>0.625</v>
+      </c>
+      <c r="Q25" s="7">
+        <f>K25/6</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="R25" s="7"/>
       <c r="AY25" s="2"/>
       <c r="AZ25" s="2"/>
       <c r="BA25" s="2"/>
       <c r="BB25" s="2"/>
       <c r="BC25" s="2"/>
-    </row>
-    <row r="26" spans="2:55" ht="16.8">
+      <c r="BD25" s="2"/>
+    </row>
+    <row r="26" spans="2:56" ht="18" thickTop="1" thickBot="1">
       <c r="B26">
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" t="s">
         <v>11</v>
-      </c>
-      <c r="E26" t="s">
-        <v>9</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
       </c>
       <c r="G26" t="s">
-        <v>10</v>
-      </c>
-      <c r="AX26" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J26" s="9">
+        <v>3</v>
+      </c>
+      <c r="K26" s="9">
+        <v>5</v>
+      </c>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="O26" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P26" s="7">
+        <f>J26/8</f>
+        <v>0.375</v>
+      </c>
+      <c r="Q26" s="7">
+        <f>K26/6</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="R26" s="7"/>
       <c r="AY26" s="2"/>
       <c r="AZ26" s="2"/>
       <c r="BA26" s="2"/>
       <c r="BB26" s="2"/>
       <c r="BC26" s="2"/>
-    </row>
-    <row r="27" spans="2:55" ht="16.8">
+      <c r="BD26" s="2"/>
+    </row>
+    <row r="27" spans="2:56" ht="18" thickTop="1" thickBot="1">
       <c r="B27">
         <v>8</v>
       </c>
       <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" t="s">
         <v>12</v>
       </c>
-      <c r="D27" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" t="s">
-        <v>6</v>
-      </c>
       <c r="G27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AX27" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
       <c r="AY27" s="2"/>
       <c r="AZ27" s="2"/>
       <c r="BA27" s="2"/>
       <c r="BB27" s="2"/>
       <c r="BC27" s="2"/>
-    </row>
-    <row r="28" spans="2:55" ht="16.8">
+      <c r="BD27" s="2"/>
+    </row>
+    <row r="28" spans="2:56" ht="18" thickTop="1" thickBot="1">
       <c r="B28">
         <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F28" t="s">
         <v>8</v>
       </c>
       <c r="G28" t="s">
-        <v>7</v>
-      </c>
-      <c r="AX28" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="O28" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P28" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q28" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R28" s="7"/>
       <c r="AY28" s="2"/>
       <c r="AZ28" s="2"/>
       <c r="BA28" s="2"/>
       <c r="BB28" s="2"/>
       <c r="BC28" s="2"/>
-    </row>
-    <row r="29" spans="2:55" ht="16.8">
+      <c r="BD28" s="2"/>
+    </row>
+    <row r="29" spans="2:56" ht="18" thickTop="1" thickBot="1">
       <c r="B29">
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F29" t="s">
         <v>8</v>
       </c>
       <c r="G29" t="s">
-        <v>10</v>
-      </c>
-      <c r="AX29" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J29" s="10">
+        <v>5</v>
+      </c>
+      <c r="K29" s="9">
+        <v>1</v>
+      </c>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="O29" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="P29" s="8">
+        <f>J29/7</f>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="Q29" s="7">
+        <f>K29/7</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="R29" s="7"/>
       <c r="AY29" s="2"/>
       <c r="AZ29" s="2"/>
       <c r="BA29" s="2"/>
       <c r="BB29" s="2"/>
       <c r="BC29" s="2"/>
-    </row>
-    <row r="30" spans="2:55">
+      <c r="BD29" s="2"/>
+    </row>
+    <row r="30" spans="2:56" ht="15.6" thickTop="1" thickBot="1">
       <c r="B30">
         <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F30" t="s">
         <v>8</v>
       </c>
       <c r="G30" t="s">
-        <v>7</v>
-      </c>
-      <c r="I30" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="2:55">
+        <v>23</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J30" s="9">
+        <v>2</v>
+      </c>
+      <c r="K30" s="9">
+        <v>6</v>
+      </c>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="O30" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P30" s="7">
+        <f>J30/7</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="Q30" s="7">
+        <f>K30/7</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="R30" s="7"/>
+    </row>
+    <row r="31" spans="2:56" ht="15.6" thickTop="1" thickBot="1">
       <c r="B31">
         <v>12</v>
       </c>
       <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" t="s">
         <v>11</v>
-      </c>
-      <c r="D31" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" t="s">
-        <v>9</v>
       </c>
       <c r="F31" t="s">
         <v>8</v>
       </c>
       <c r="G31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="2:55">
+        <v>30</v>
+      </c>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+    </row>
+    <row r="32" spans="2:56" ht="15.6" thickTop="1" thickBot="1">
       <c r="B32">
         <v>13</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F32" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G32" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7">
+        <v>30</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="K32" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="O32" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q32" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="R32" s="7"/>
+    </row>
+    <row r="33" spans="2:18" ht="15.6" thickTop="1" thickBot="1">
       <c r="B33">
         <v>14</v>
       </c>
       <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" t="s">
         <v>11</v>
-      </c>
-      <c r="D33" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" t="s">
-        <v>9</v>
       </c>
       <c r="F33" t="s">
         <v>8</v>
       </c>
       <c r="G33" t="s">
-        <v>10</v>
+        <v>30</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J33" s="9">
+        <v>5</v>
+      </c>
+      <c r="K33" s="9">
+        <v>1</v>
+      </c>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="O33" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="P33" s="7">
+        <f>J33/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q33" s="7">
+        <f>K33/4</f>
+        <v>0.25</v>
+      </c>
+      <c r="R33" s="7"/>
+    </row>
+    <row r="34" spans="2:18" ht="15.6" thickTop="1" thickBot="1">
+      <c r="I34" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J34" s="9">
+        <v>5</v>
+      </c>
+      <c r="K34" s="9">
+        <v>3</v>
+      </c>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="O34" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P34" s="7">
+        <f>J34/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q34" s="7">
+        <f>K34/4</f>
+        <v>0.75</v>
+      </c>
+      <c r="R34" s="7"/>
+    </row>
+    <row r="35" spans="2:18" ht="15" thickTop="1">
+      <c r="J35">
+        <f>SUM(J34,J33,J30,J29,J26,J25,J22,J21,)/14</f>
+        <v>2.1428571428571428</v>
+      </c>
+      <c r="K35">
+        <f>SUM(K34,K33,K30,K29,K26,K25,K22,K21,)/14</f>
+        <v>1.5714285714285714</v>
+      </c>
+      <c r="M35">
+        <f>SUM(M21:M34)/14</f>
+        <v>3.8571428571428572</v>
+      </c>
+    </row>
+    <row r="38" spans="2:18">
+      <c r="B38" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K38" t="s">
+        <v>38</v>
+      </c>
+      <c r="L38">
+        <f>8/14</f>
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" ht="15" thickBot="1">
+      <c r="B39" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" t="s">
+        <v>40</v>
+      </c>
+      <c r="K39" t="s">
+        <v>41</v>
+      </c>
+      <c r="L39">
+        <f>6/14</f>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="40" spans="2:18" ht="15" thickBot="1">
+      <c r="B40" s="12"/>
+      <c r="C40" t="s">
+        <v>42</v>
+      </c>
+      <c r="J40" s="12"/>
+      <c r="K40" s="11"/>
+    </row>
+    <row r="41" spans="2:18" ht="15" thickBot="1">
+      <c r="J41" s="12"/>
+      <c r="K41" t="s">
+        <v>43</v>
+      </c>
+      <c r="L41" s="12">
+        <f>6/14</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="M41" s="13"/>
+    </row>
+    <row r="42" spans="2:18" ht="15" thickBot="1">
+      <c r="C42" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42">
+        <f>L50*P21*P25*P29*P33</f>
+        <v>5.7397959183673464E-2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>45</v>
+      </c>
+      <c r="J42" s="12"/>
+      <c r="K42" t="s">
+        <v>46</v>
+      </c>
+      <c r="L42" s="15">
+        <f>8/14</f>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="M42" s="13"/>
+    </row>
+    <row r="43" spans="2:18" ht="15" thickBot="1">
+      <c r="C43" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43">
+        <f>L51*P34*P30*P26*P22</f>
+        <v>1.020408163265306E-2</v>
+      </c>
+      <c r="J43" s="12"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="12"/>
+      <c r="M43" s="13"/>
+    </row>
+    <row r="44" spans="2:18" ht="15" thickBot="1">
+      <c r="J44" s="12"/>
+      <c r="K44" t="s">
+        <v>48</v>
+      </c>
+      <c r="L44" s="12">
+        <f>6/14</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="M44" s="13"/>
+    </row>
+    <row r="45" spans="2:18" ht="15" thickBot="1">
+      <c r="B45" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" t="s">
+        <v>50</v>
+      </c>
+      <c r="J45" s="12"/>
+      <c r="K45" t="s">
+        <v>51</v>
+      </c>
+      <c r="L45" s="12">
+        <f>8/14</f>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="M45" s="13"/>
+    </row>
+    <row r="46" spans="2:18">
+      <c r="C46" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="2:18">
+      <c r="K47" t="s">
+        <v>53</v>
+      </c>
+      <c r="L47">
+        <f>6/14</f>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="48" spans="2:18">
+      <c r="C48" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48">
+        <f>L50*Q21*Q25*P29*Q33</f>
+        <v>5.1020408163265302E-3</v>
+      </c>
+      <c r="F48" t="s">
+        <v>54</v>
+      </c>
+      <c r="K48" t="s">
+        <v>55</v>
+      </c>
+      <c r="L48">
+        <f>8/14</f>
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12">
+      <c r="C49" t="s">
+        <v>47</v>
+      </c>
+      <c r="D49">
+        <f>L51*Q22*Q26*P30*Q34</f>
+        <v>6.1224489795918366E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12">
+      <c r="K50" t="s">
+        <v>56</v>
+      </c>
+      <c r="L50">
+        <f>6/14</f>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12">
+      <c r="B51" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51" t="s">
+        <v>58</v>
+      </c>
+      <c r="K51" t="s">
+        <v>59</v>
+      </c>
+      <c r="L51" s="6">
+        <f>8/14</f>
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12">
+      <c r="C52" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12">
+      <c r="C54" t="s">
+        <v>44</v>
+      </c>
+      <c r="D54">
+        <f>L50*R21*P25*Q29*Q33</f>
+        <v>2.3915816326530608E-3</v>
+      </c>
+      <c r="F54" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12">
+      <c r="C55" t="s">
+        <v>47</v>
+      </c>
+      <c r="D55">
+        <f>L51*R22*P26*Q30*Q34</f>
+        <v>3.4438775510204078E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="B6:G8"/>
-    <mergeCell ref="I17:O18"/>
     <mergeCell ref="B10:D11"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="O19:Q19"/>
+    <mergeCell ref="I17:R18"/>
+    <mergeCell ref="B17:G18"/>
   </mergeCells>
-  <dataValidations count="4">
+  <dataValidations disablePrompts="1" count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20:C33" xr:uid="{84C8BB0A-8D5C-4606-893A-35D68D72B48C}">
       <formula1>$B$13:$B$15</formula1>
     </dataValidation>

</xml_diff>